<commit_message>
added name and conditional hiding
</commit_message>
<xml_diff>
--- a/144F20/Topic 5/QR 3-3 Tech Template Modified.xlsx
+++ b/144F20/Topic 5/QR 3-3 Tech Template Modified.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.ketchersid\OneDrive - GCU Employees\Course Materials\git\Teaching\144F20\Topic 5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gcumail-my.sharepoint.com/personal/richard_ketchersid_gcu_edu/Documents/Course Materials/git/Teaching/144F20/Topic 5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73523178-FF91-4772-A983-A9420069EC9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:80_{E9FF61AF-2872-432F-9DF8-BF4D9D52450F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="19272" windowHeight="11400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="960" windowWidth="24090" windowHeight="14250" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Games" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
   <si>
     <t>Game</t>
   </si>
@@ -209,6 +209,12 @@
       <t>.</t>
     </r>
   </si>
+  <si>
+    <t>Enter Name  ⇒</t>
+  </si>
+  <si>
+    <t>Your Name Here</t>
+  </si>
 </sst>
 </file>
 
@@ -217,7 +223,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000%"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -313,8 +319,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Bradley Hand ITC"/>
+      <family val="4"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,8 +378,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -622,11 +655,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -916,12 +964,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -955,13 +1025,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>784860</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>198120</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1008,8 +1078,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{46848E41-8427-4151-B667-C51179324944}">
-  <header guid="{46848E41-8427-4151-B667-C51179324944}" dateTime="2020-12-08T15:38:29" maxSheetId="3" userName="Richard Ketchersid" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FCF5FE3F-8619-44EE-90BF-4B9C59A69FF0}">
+  <header guid="{FCF5FE3F-8619-44EE-90BF-4B9C59A69FF0}" dateTime="2022-05-05T12:28:46" maxSheetId="3" userName="Richard Ketchersid" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1024,7 +1094,7 @@
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{46848E41-8427-4151-B667-C51179324944}" name="Richard Ketchersid" id="-1739565536" dateTime="2020-12-08T15:38:29"/>
+  <userInfo guid="{FCF5FE3F-8619-44EE-90BF-4B9C59A69FF0}" name="Richard Ketchersid" id="-1739543589" dateTime="2022-05-05T12:28:46"/>
 </users>
 </file>
 
@@ -1291,279 +1361,296 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="71.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="21.8984375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="24.59765625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="18.69921875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="25.796875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.69921875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.19921875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.69921875" customWidth="1"/>
-    <col min="9" max="9" width="34.09765625" style="23" customWidth="1"/>
-    <col min="10" max="10" width="20.8984375" customWidth="1"/>
-    <col min="11" max="11" width="23.296875" customWidth="1"/>
+    <col min="2" max="2" width="21.875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="24.625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18.75" style="4" customWidth="1"/>
+    <col min="5" max="5" width="25.75" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.75" customWidth="1"/>
+    <col min="9" max="9" width="34.125" style="23" customWidth="1"/>
+    <col min="10" max="10" width="20.875" customWidth="1"/>
+    <col min="11" max="11" width="23.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="70" t="s">
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="84" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="86" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="83"/>
+    </row>
+    <row r="4" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="71"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="78" t="s">
+      <c r="C4" s="71"/>
+    </row>
+    <row r="5" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B5" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C5" s="26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="79"/>
-      <c r="B4" s="27" t="s">
+    <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="79"/>
+      <c r="B6" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C6" s="28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="80"/>
-      <c r="B5" s="29" t="s">
+      <c r="F6" s="85"/>
+    </row>
+    <row r="7" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="80"/>
+      <c r="B7" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C7" s="30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="31" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C8" s="30" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="32" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C9" s="30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="33" t="s">
+    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C10" s="34" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+    <row r="13" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D13" s="13">
         <f>PERMUT(20,2)</f>
         <v>380</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F13" s="11">
         <v>1</v>
       </c>
-      <c r="G11" s="18">
-        <f>F11/D11</f>
+      <c r="G13" s="18">
+        <f>F13/D13</f>
         <v>2.631578947368421E-3</v>
       </c>
-      <c r="H11" s="11">
-        <f>(1-G11)/G11</f>
+      <c r="H13" s="11">
+        <f>(1-G13)/G13</f>
         <v>379</v>
       </c>
-      <c r="I11" s="6" t="str">
-        <f>"Your odds of winning are "&amp;H11&amp;" to 1!"</f>
+      <c r="I13" s="6" t="str">
+        <f>"Your odds of winning are "&amp;H13&amp;" to 1!"</f>
         <v>Your odds of winning are 379 to 1!</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+    <row r="14" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="6" t="str">
-        <f>"Your odds of winning are "&amp;IF(NOT(ISBLANK(H12)),H12,"???")&amp;" to 1!"</f>
-        <v>Your odds of winning are ??? to 1!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="6" t="str">
-        <f t="shared" ref="I13:I15" si="0">"Your odds of winning are "&amp;IF(NOT(ISBLANK(H13)),H13,"???")&amp;" to 1!"</f>
-        <v>Your odds of winning are ??? to 1!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="9"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="17"/>
       <c r="G14" s="19"/>
       <c r="H14" s="12"/>
       <c r="I14" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f>"Your odds of winning are "&amp;IF(NOT(ISBLANK(H14)),H14,"???")&amp;" to 1!"</f>
         <v>Your odds of winning are ??? to 1!</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="9"/>
+    <row r="15" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="35"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="8"/>
       <c r="F15" s="17"/>
       <c r="G15" s="19"/>
       <c r="H15" s="12"/>
       <c r="I15" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I15:I17" si="0">"Your odds of winning are "&amp;IF(NOT(ISBLANK(H15)),H15,"???")&amp;" to 1!"</f>
         <v>Your odds of winning are ??? to 1!</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="12"/>
+    <row r="16" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="36"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="19"/>
       <c r="H16" s="12"/>
       <c r="I16" s="6" t="str">
-        <f>"Your odds of winning are "&amp;IF(NOT(ISBLANK(H16)),ROUND(H16,0),"???")&amp;" to 1!"</f>
+        <f t="shared" si="0"/>
         <v>Your odds of winning are ??? to 1!</v>
       </c>
     </row>
-    <row r="17" spans="6:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F18" s="72" t="s">
+    <row r="17" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="36"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Your odds of winning are ??? to 1!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="37"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="6" t="str">
+        <f>"Your odds of winning are "&amp;IF(NOT(ISBLANK(H18)),ROUND(H18,0),"???")&amp;" to 1!"</f>
+        <v>Your odds of winning are ??? to 1!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F20" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="73"/>
-    </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F19" s="74"/>
-      <c r="G19" s="75"/>
-    </row>
-    <row r="20" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F20" s="74"/>
-      <c r="G20" s="75"/>
-    </row>
-    <row r="21" spans="6:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F21" s="76"/>
-      <c r="G21" s="77"/>
-    </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="G22" s="3"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B44" s="24" t="s">
+      <c r="G20" s="73"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F21" s="74"/>
+      <c r="G21" s="75"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F22" s="74"/>
+      <c r="G22" s="75"/>
+    </row>
+    <row r="23" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="76"/>
+      <c r="G23" s="77"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G24" s="3"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B45" s="24" t="s">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="24" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{13B6492D-170C-45E1-97D8-793CC53D410C}" showRuler="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E7" sqref="E7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="3">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F18:G21"/>
-    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F20:G23"/>
+    <mergeCell ref="A5:A7"/>
   </mergeCells>
+  <conditionalFormatting sqref="A3:I23">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$C$2="Your Name Here"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" error="Make a selection" promptTitle="Choose" prompt="Permutation_x000a_Combination" sqref="B12:B16" xr:uid="{F1371D0C-4D6C-4564-8606-B5780CB0D4F2}">
-      <formula1>$B$44:$B$45</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" error="Make a selection" promptTitle="Choose" prompt="Permutation_x000a_Combination" sqref="B14:B18" xr:uid="{F1371D0C-4D6C-4564-8606-B5780CB0D4F2}">
+      <formula1>$B$46:$B$47</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1573,8 +1660,8 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{495C08AE-80E7-4948-9AA1-572EA21DB2FC}">
-            <xm:f>B12&lt;&gt;soln1!B11</xm:f>
+          <x14:cfRule type="expression" priority="3" id="{495C08AE-80E7-4948-9AA1-572EA21DB2FC}">
+            <xm:f>B14&lt;&gt;soln1!B11</xm:f>
             <x14:dxf>
               <font>
                 <b/>
@@ -1583,8 +1670,8 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="2" id="{5DAB86F2-292A-45BF-AB02-5BA097126ADD}">
-            <xm:f>B12=soln1!B11</xm:f>
+          <x14:cfRule type="expression" priority="4" id="{5DAB86F2-292A-45BF-AB02-5BA097126ADD}">
+            <xm:f>B14=soln1!B11</xm:f>
             <x14:dxf>
               <font>
                 <b/>
@@ -1593,7 +1680,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B12:B16 D12:D16 F12:H16</xm:sqref>
+          <xm:sqref>B14:B18 D14:D18 F14:H18</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1609,30 +1696,30 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="71.5" style="38" customWidth="1"/>
-    <col min="2" max="2" width="21.8984375" style="38" customWidth="1"/>
-    <col min="3" max="3" width="24.59765625" style="38" customWidth="1"/>
-    <col min="4" max="4" width="18.69921875" style="38" customWidth="1"/>
-    <col min="5" max="5" width="25.796875" style="38" customWidth="1"/>
-    <col min="6" max="6" width="18.69921875" style="39" customWidth="1"/>
-    <col min="7" max="7" width="18.19921875" style="39" customWidth="1"/>
-    <col min="8" max="8" width="15.69921875" style="40" customWidth="1"/>
-    <col min="9" max="9" width="34.09765625" style="41" customWidth="1"/>
-    <col min="10" max="10" width="20.8984375" style="40" customWidth="1"/>
-    <col min="11" max="11" width="23.296875" style="40" customWidth="1"/>
+    <col min="2" max="2" width="21.875" style="38" customWidth="1"/>
+    <col min="3" max="3" width="24.625" style="38" customWidth="1"/>
+    <col min="4" max="4" width="18.75" style="38" customWidth="1"/>
+    <col min="5" max="5" width="25.75" style="38" customWidth="1"/>
+    <col min="6" max="6" width="18.75" style="39" customWidth="1"/>
+    <col min="7" max="7" width="18.25" style="39" customWidth="1"/>
+    <col min="8" max="8" width="15.75" style="40" customWidth="1"/>
+    <col min="9" max="9" width="34.125" style="41" customWidth="1"/>
+    <col min="10" max="10" width="20.875" style="40" customWidth="1"/>
+    <col min="11" max="11" width="23.25" style="40" customWidth="1"/>
     <col min="12" max="16384" width="11" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:9" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="81" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="82"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="42" t="s">
         <v>14</v>
       </c>
@@ -1640,7 +1727,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="44" t="s">
         <v>16</v>
       </c>
@@ -1648,7 +1735,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="46" t="s">
         <v>18</v>
       </c>
@@ -1656,7 +1743,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="47" t="s">
         <v>20</v>
       </c>
@@ -1664,7 +1751,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="48" t="s">
         <v>22</v>
       </c>
@@ -1672,8 +1759,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:9" s="52" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:9" s="52" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
         <v>0</v>
       </c>
@@ -1702,7 +1789,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="53" t="s">
         <v>4</v>
       </c>
@@ -1735,7 +1822,7 @@
         <v>Your odds of winning are 379 to 1!</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
         <v>5</v>
       </c>
@@ -1768,7 +1855,7 @@
         <v>Your odds of winning are 1 to 6839!</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>6</v>
       </c>
@@ -1801,7 +1888,7 @@
         <v>Your odds of winning are 1 to 116279!</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="64" t="s">
         <v>2</v>
       </c>
@@ -1834,7 +1921,7 @@
         <v>Your odds of winning are 1 to 5527199!</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="64" t="s">
         <v>3</v>
       </c>
@@ -1867,7 +1954,7 @@
         <v>Your odds of winning are 1 to 658007!</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="67" t="s">
         <v>27</v>
       </c>
@@ -1901,22 +1988,22 @@
         <v>Your odds of winning are 1 to 109.589579831933!</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G16" s="69"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G17" s="69"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G18" s="69"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G19" s="69"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G20" s="69"/>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G21" s="69"/>
     </row>
   </sheetData>

</xml_diff>